<commit_message>
#CRM-1168 Add brand column in Partner panel - Pending Spares - Download file
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27F8325-F17A-44A8-8871-1F26FEA30C17}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Customer Name</t>
   </si>
@@ -95,25 +104,36 @@
   </si>
   <si>
     <t>{spare:gst_no}</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>{spare:brands}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF4B5056"/>
       <name val="Helvetica Neue"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Cambria"/>
     </font>
   </fonts>
@@ -122,7 +142,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -132,50 +152,368 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="14.43"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -218,8 +556,11 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -262,21 +603,24 @@
       <c r="N2" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1262,6 +1606,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Service Center Poc Phone number in the Spare requested excel sheet	 #CRM-1338
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27F8325-F17A-44A8-8871-1F26FEA30C17}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Customer Name</t>
   </si>
@@ -49,6 +40,9 @@
     <t>Service Center Name</t>
   </si>
   <si>
+    <t>Service Center Mobile No</t>
+  </si>
+  <si>
     <t>Service Center Address</t>
   </si>
   <si>
@@ -64,6 +58,9 @@
     <t>Service Center GST Number</t>
   </si>
   <si>
+    <t>Brand</t>
+  </si>
+  <si>
     <t>{spare:name}</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
     <t>{spare:vendor_name}</t>
   </si>
   <si>
+    <t>{spare:primary_contact_phone_1}</t>
+  </si>
+  <si>
     <t>{spare:address}</t>
   </si>
   <si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>{spare:gst_no}</t>
-  </si>
-  <si>
-    <t>Brand</t>
   </si>
   <si>
     <t>{spare:brands}</t>
@@ -115,26 +112,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF4B5056"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -142,7 +144,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -151,369 +153,76 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="15.57"/>
+    <col customWidth="1" min="2" max="2" width="23.57"/>
+    <col customWidth="1" min="3" max="3" width="16.0"/>
+    <col customWidth="1" min="4" max="4" width="18.86"/>
+    <col customWidth="1" min="5" max="5" width="19.86"/>
+    <col customWidth="1" min="6" max="6" width="19.29"/>
+    <col customWidth="1" min="7" max="7" width="18.71"/>
+    <col customWidth="1" min="8" max="8" width="19.71"/>
+    <col customWidth="1" min="9" max="10" width="20.57"/>
+    <col customWidth="1" min="11" max="11" width="22.57"/>
+    <col customWidth="1" min="12" max="12" width="21.57"/>
+    <col customWidth="1" min="13" max="13" width="22.86"/>
+    <col customWidth="1" min="14" max="14" width="20.0"/>
+    <col customWidth="1" min="15" max="15" width="24.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +250,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -553,74 +262,80 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="N2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1606,6 +1321,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRM-1761 Add customer mobile no in pending booking and panding spare on partner pannel
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55690307-9995-4470-A4DF-261D1D9A5383}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Customer Name</t>
   </si>
@@ -107,35 +116,41 @@
   </si>
   <si>
     <t>{spare:brands}</t>
+  </si>
+  <si>
+    <t>Customer Phone Number</t>
+  </si>
+  <si>
+    <t>{spare:customer_mobile}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF4B5056"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -144,7 +159,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -154,188 +169,501 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.57"/>
-    <col customWidth="1" min="2" max="2" width="23.57"/>
-    <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="4" width="18.86"/>
-    <col customWidth="1" min="5" max="5" width="19.86"/>
-    <col customWidth="1" min="6" max="6" width="19.29"/>
-    <col customWidth="1" min="7" max="7" width="18.71"/>
-    <col customWidth="1" min="8" max="8" width="19.71"/>
-    <col customWidth="1" min="9" max="10" width="20.57"/>
-    <col customWidth="1" min="11" max="11" width="22.57"/>
-    <col customWidth="1" min="12" max="12" width="21.57"/>
-    <col customWidth="1" min="13" max="13" width="22.86"/>
-    <col customWidth="1" min="14" max="14" width="20.0"/>
-    <col customWidth="1" min="15" max="15" width="24.71"/>
+    <col min="1" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="11" width="20.5546875" customWidth="1"/>
+    <col min="12" max="12" width="22.5546875" customWidth="1"/>
+    <col min="13" max="13" width="21.5546875" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1321,9 +1649,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Part Code in the spare download excel file #CRM-2487
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55690307-9995-4470-A4DF-261D1D9A5383}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Customer Name</t>
   </si>
   <si>
+    <t>Customer Phone Number</t>
+  </si>
+  <si>
     <t>Invoice Id</t>
   </si>
   <si>
@@ -34,6 +28,9 @@
     <t>Age of Requested</t>
   </si>
   <si>
+    <t>Parts Code</t>
+  </si>
+  <si>
     <t>Parts Required</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
     <t>{spare:name}</t>
   </si>
   <si>
+    <t>{spare:customer_mobile}</t>
+  </si>
+  <si>
     <t>{spare:purchase_invoice_id}</t>
   </si>
   <si>
@@ -82,6 +82,9 @@
     <t>{spare:age_of_request}</t>
   </si>
   <si>
+    <t>{spare:part_number}</t>
+  </si>
+  <si>
     <t>{spare:parts_requested}</t>
   </si>
   <si>
@@ -116,41 +119,35 @@
   </si>
   <si>
     <t>{spare:brands}</t>
-  </si>
-  <si>
-    <t>Customer Phone Number</t>
-  </si>
-  <si>
-    <t>{spare:customer_mobile}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF4B5056"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -159,7 +156,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -169,501 +166,199 @@
     </fill>
   </fills>
   <borders count="2">
+    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="10" max="11" width="20.5546875" customWidth="1"/>
-    <col min="12" max="12" width="22.5546875" customWidth="1"/>
-    <col min="13" max="13" width="21.5546875" customWidth="1"/>
-    <col min="14" max="14" width="22.88671875" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="24.6640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="15.57"/>
+    <col customWidth="1" min="3" max="3" width="23.57"/>
+    <col customWidth="1" min="4" max="4" width="16.0"/>
+    <col customWidth="1" min="5" max="5" width="18.86"/>
+    <col customWidth="1" min="6" max="7" width="19.86"/>
+    <col customWidth="1" min="8" max="8" width="19.29"/>
+    <col customWidth="1" min="9" max="9" width="18.71"/>
+    <col customWidth="1" min="10" max="10" width="19.71"/>
+    <col customWidth="1" min="11" max="12" width="20.57"/>
+    <col customWidth="1" min="13" max="13" width="22.57"/>
+    <col customWidth="1" min="14" max="14" width="21.57"/>
+    <col customWidth="1" min="15" max="15" width="22.86"/>
+    <col customWidth="1" min="16" max="16" width="20.0"/>
+    <col customWidth="1" min="17" max="17" width="24.71"/>
+    <col customWidth="1" min="18" max="18" width="14.43"/>
+    <col customWidth="1" min="19" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
+      <c r="P2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1"/>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1649,7 +1344,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add requested quantity & shipped quantity in the Partner Panel spare report #CRM-4144
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Requested_Parts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Customer Name</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Parts Required</t>
   </si>
   <si>
+    <t xml:space="preserve">Parts Quantity</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model Number</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">{spare:parts_requested}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare:quantity}</t>
   </si>
   <si>
     <t xml:space="preserve">{spare:model_number}</t>
@@ -149,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -192,6 +198,11 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -248,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +277,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,29 +361,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1000"/>
+  <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="21" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="22" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -426,73 +441,79 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="I2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>39</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>